<commit_message>
docs(logging): update Mouad time logging
</commit_message>
<xml_diff>
--- a/Zeitlogging/Mouad.xlsx
+++ b/Zeitlogging/Mouad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school\Modul-324\Zeitlogging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F6C3DD8-EEF7-4F99-8D1F-D0ECF1106231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E736925-A350-4681-9BA2-B506BF76AA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Erfassung" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Datum</t>
   </si>
@@ -57,10 +56,22 @@
     <t>Projekt/Kommentar</t>
   </si>
   <si>
-    <t>XY-Bericht schreiben</t>
+    <t>Einführung DevOps + Modulstart</t>
   </si>
   <si>
-    <t>Bericht Projekt A</t>
+    <t>Theorieteil DevOps</t>
+  </si>
+  <si>
+    <t>Lernjournal Vorlage &amp; Excel Zeitlogging</t>
+  </si>
+  <si>
+    <t>Projektstruktur &amp; Repo</t>
+  </si>
+  <si>
+    <t>Dokumentationsstruktur</t>
+  </si>
+  <si>
+    <t>P1 Aufgabe lesen &amp; Einrichten</t>
   </si>
 </sst>
 </file>
@@ -68,8 +79,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="dd\.mm\.yyyy"/>
-    <numFmt numFmtId="166" formatCode="[h]:mm"/>
+    <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
+    <numFmt numFmtId="165" formatCode="[h]:mm"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -135,18 +146,18 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2"/>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="2"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="2"/>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="2"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="2"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1"/>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="2" xfId="2"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="3"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="3"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="date_swiss" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -481,13 +492,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
@@ -529,32 +540,66 @@
         <v>0.34027777777777779</v>
       </c>
       <c r="D2" s="3">
-        <v>0.37152777777777779</v>
+        <v>0.40972222222222221</v>
       </c>
       <c r="E2" s="3">
-        <v>0</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="F2" s="4">
         <f t="shared" ref="F2:F65" si="0">IF(AND(C2&lt;&gt;"",D2&lt;&gt;""),D2-C2-IF(E2="",0,E2),"")</f>
-        <v>3.125E-2</v>
+        <v>6.2499999999999972E-2</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
+      <c r="A3" s="2">
+        <v>45891</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.40972222222222221</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="F3" s="4">
+        <f t="shared" si="0"/>
+        <v>3.1250000000000007E-2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
+      <c r="A4" s="2">
+        <v>45891</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="E4" s="3">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="F4" s="4">
+        <f t="shared" si="0"/>
+        <v>3.1250000000000028E-2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -10132,7 +10177,7 @@
       <c r="D962" s="3"/>
       <c r="E962" s="3"/>
       <c r="F962" s="4" t="str">
-        <f t="shared" ref="F962:F1025" si="15">IF(AND(C962&lt;&gt;"",D962&lt;&gt;""),D962-C962-IF(E962="",0,E962),"")</f>
+        <f t="shared" ref="F962:F1001" si="15">IF(AND(C962&lt;&gt;"",D962&lt;&gt;""),D962-C962-IF(E962="",0,E962),"")</f>
         <v/>
       </c>
     </row>
@@ -10533,7 +10578,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Zeitformat" prompt="Bitte Zeit als HH:MM eingeben (z.B. 08:30)." sqref="C2:C1001 D2:D1001 E2:E1001" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Zeitformat" prompt="Bitte Zeit als HH:MM eingeben (z.B. 08:30)." sqref="C2:E1001" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>TIME(0,0,0)</formula1>
       <formula2>TIME(23,59,59)</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
chore: update Mouad.xlsx file
</commit_message>
<xml_diff>
--- a/Zeitlogging/Mouad.xlsx
+++ b/Zeitlogging/Mouad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school\Modul-324\Zeitlogging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E736925-A350-4681-9BA2-B506BF76AA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DD12AC-EDA9-4894-966E-B81427C9634E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,13 +65,13 @@
     <t>Lernjournal Vorlage &amp; Excel Zeitlogging</t>
   </si>
   <si>
-    <t>Projektstruktur &amp; Repo</t>
-  </si>
-  <si>
     <t>Dokumentationsstruktur</t>
   </si>
   <si>
     <t>P1 Aufgabe lesen &amp; Einrichten</t>
+  </si>
+  <si>
+    <t>Einrichtung Gruppenrepo &amp; persönliches Repo</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -503,7 +503,7 @@
     <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -558,7 +558,7 @@
         <v>45891</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3">
         <v>0.40972222222222221</v>
@@ -574,7 +574,7 @@
         <v>3.1250000000000007E-2</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -598,7 +598,7 @@
         <v>3.1250000000000028E-2</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
chore: update Mouad.xlsx with latest time logging data
</commit_message>
<xml_diff>
--- a/Zeitlogging/Mouad.xlsx
+++ b/Zeitlogging/Mouad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school\Modul-324\Zeitlogging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DD12AC-EDA9-4894-966E-B81427C9634E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473FE485-7FE4-4C67-8ACA-47FEAC3FFAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Datum</t>
   </si>
@@ -68,10 +68,34 @@
     <t>Dokumentationsstruktur</t>
   </si>
   <si>
-    <t>P1 Aufgabe lesen &amp; Einrichten</t>
+    <t>Einrichtung Gruppenrepo &amp; persönliches Repo</t>
   </si>
   <si>
-    <t>Einrichtung Gruppenrepo &amp; persönliches Repo</t>
+    <t>T2 – Theorie The Three Ways</t>
+  </si>
+  <si>
+    <t>Einlesen und Beantworten von Fragen</t>
+  </si>
+  <si>
+    <t>Meeting</t>
+  </si>
+  <si>
+    <t>Feedback &amp; Update</t>
+  </si>
+  <si>
+    <t>P1 – Aufgabe lesen &amp; Einrichten</t>
+  </si>
+  <si>
+    <t>T3 – Aufgabe lesen</t>
+  </si>
+  <si>
+    <t>T3 – Recherche</t>
+  </si>
+  <si>
+    <t>Recherche und Beantwortung der Fragen</t>
+  </si>
+  <si>
+    <t>Sich einlesen &amp; einarbeiten</t>
   </si>
 </sst>
 </file>
@@ -150,7 +174,7 @@
     <xf numFmtId="20" fontId="2" fillId="0" borderId="2"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -158,6 +182,8 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1"/>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="2" xfId="2"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="3"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="date_swiss" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -492,7 +518,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -558,7 +584,7 @@
         <v>45891</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3">
         <v>0.40972222222222221</v>
@@ -574,7 +600,7 @@
         <v>3.1250000000000007E-2</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -602,43 +628,99 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4" t="str">
+      <c r="A5" s="2">
+        <v>45898</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.40972222222222221</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F5" s="4">
         <f t="shared" si="0"/>
-        <v/>
+        <v>4.8611111111111091E-2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A6" s="5">
+        <v>45898</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.40972222222222221</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0.43402777777777779</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <f>IF(AND(C6&lt;&gt;"",D6&lt;&gt;""),D6-C6-IF(E6="",0,E6),"")</f>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A7" s="2">
+        <v>45898</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.43402777777777779</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.44097222222222221</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <f>IF(AND(C7&lt;&gt;"",D7&lt;&gt;""),D7-C7-IF(E7="",0,E7),"")</f>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="A8" s="2">
+        <v>45898</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.44097222222222221</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="E8" s="3">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="F8" s="4">
+        <f>IF(AND(C8&lt;&gt;"",D8&lt;&gt;""),D8-C8-IF(E8="",0,E8),"")</f>
+        <v>4.5138888888888923E-2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -10578,11 +10660,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Zeitformat" prompt="Bitte Zeit als HH:MM eingeben (z.B. 08:30)." sqref="C2:E1001" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Zeitformat" prompt="Bitte Zeit als HH:MM eingeben (z.B. 08:30)." sqref="C2:E5 C7:E1001" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>TIME(0,0,0)</formula1>
       <formula2>TIME(23,59,59)</formula2>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Datum" prompt="Bitte Datum eingeben (TT.MM.JJJJ)." sqref="A2:A1001" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Datum" prompt="Bitte Datum eingeben (TT.MM.JJJJ)." sqref="A2:A5 A7:A1001" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>DATE(2000,1,1)</formula1>
       <formula2>DATE(2100,12,31)</formula2>
     </dataValidation>

</xml_diff>